<commit_message>
Updated LUA to roll Task and Challenge dice.
</commit_message>
<xml_diff>
--- a/To-Do.xlsx
+++ b/To-Do.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tomaw\AppData\Roaming\Fantasy Grounds\rulesets\Star Trek Adventures\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{04F54153-D5E6-494F-A94D-1197107C893B}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B208D861-FC30-4FB0-B534-F8016C6D9DAA}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="750" yWindow="645" windowWidth="21600" windowHeight="11385" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1560" yWindow="1560" windowWidth="21600" windowHeight="11385" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="XML CODING" sheetId="1" r:id="rId1"/>
@@ -1456,8 +1456,8 @@
   </sheetPr>
   <dimension ref="B1:E17"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="B6" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="B4" workbookViewId="0">
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -1536,7 +1536,7 @@
     </row>
     <row r="9" spans="2:5" s="1" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B9" s="14">
-        <v>0.4</v>
+        <v>1</v>
       </c>
       <c r="C9" s="2" t="s">
         <v>29</v>
@@ -1548,7 +1548,7 @@
     </row>
     <row r="10" spans="2:5" s="1" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B10" s="14">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C10" s="2" t="s">
         <v>29</v>
@@ -1560,7 +1560,7 @@
     </row>
     <row r="11" spans="2:5" s="1" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B11" s="14">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C11" s="2" t="s">
         <v>29</v>

</xml_diff>

<commit_message>
Updated LUA to roll Reputation dice.
</commit_message>
<xml_diff>
--- a/To-Do.xlsx
+++ b/To-Do.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="21328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="21929"/>
   <workbookPr autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tomaw\AppData\Roaming\Fantasy Grounds\rulesets\Star Trek Adventures\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\wesle\AppData\Roaming\Fantasy Grounds\rulesets\Star Trek Adventures\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{610D365C-64F3-4657-A666-6882A1743C31}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{09C04869-D120-4158-AF20-A05C09B89AA3}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4140" yWindow="-14115" windowWidth="21600" windowHeight="11385" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="8556" yWindow="0" windowWidth="13116" windowHeight="12360" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="XML CODING" sheetId="1" r:id="rId1"/>
@@ -1160,18 +1160,18 @@
       <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="9.125" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="2.7109375" customWidth="1"/>
-    <col min="2" max="2" width="15.7109375" customWidth="1"/>
-    <col min="3" max="3" width="30.7109375" customWidth="1"/>
-    <col min="4" max="4" width="15.7109375" customWidth="1"/>
-    <col min="5" max="5" width="53.5703125" customWidth="1"/>
-    <col min="6" max="6" width="2.7109375" customWidth="1"/>
-    <col min="8" max="8" width="9.140625" customWidth="1"/>
+    <col min="1" max="1" width="2.75" customWidth="1"/>
+    <col min="2" max="2" width="15.75" customWidth="1"/>
+    <col min="3" max="3" width="30.75" customWidth="1"/>
+    <col min="4" max="4" width="15.75" customWidth="1"/>
+    <col min="5" max="5" width="53.625" customWidth="1"/>
+    <col min="6" max="6" width="2.75" customWidth="1"/>
+    <col min="8" max="8" width="9.125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:5" s="1" customFormat="1" ht="42.75" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="2:5" s="1" customFormat="1" ht="42.75" customHeight="1" x14ac:dyDescent="0.5">
       <c r="B1" s="9" t="s">
         <v>23</v>
       </c>
@@ -1179,8 +1179,8 @@
       <c r="D1" s="9"/>
       <c r="E1" s="9"/>
     </row>
-    <row r="2" spans="2:5" ht="15" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="3" spans="2:5" s="1" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="2:5" ht="15" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="3" spans="2:5" s="1" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B3" s="29" t="s">
         <v>0</v>
       </c>
@@ -1190,7 +1190,7 @@
       </c>
       <c r="E3" s="27"/>
     </row>
-    <row r="4" spans="2:5" s="1" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:5" s="1" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B4" s="29" t="s">
         <v>1</v>
       </c>
@@ -1198,8 +1198,8 @@
       <c r="D4" s="28"/>
       <c r="E4" s="28"/>
     </row>
-    <row r="5" spans="2:5" ht="15" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="6" spans="2:5" s="1" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:5" ht="15" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="6" spans="2:5" s="1" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B6" s="30" t="s">
         <v>24</v>
       </c>
@@ -1207,7 +1207,7 @@
       <c r="D6" s="30"/>
       <c r="E6" s="30"/>
     </row>
-    <row r="7" spans="2:5" s="1" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="2:5" s="1" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B7" s="10" t="s">
         <v>4</v>
       </c>
@@ -1221,7 +1221,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="8" spans="2:5" s="1" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="2:5" s="1" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B8" s="12">
         <f>AVERAGE(B9:B10)</f>
         <v>0.5</v>
@@ -1232,7 +1232,7 @@
       <c r="D8" s="16"/>
       <c r="E8" s="10"/>
     </row>
-    <row r="9" spans="2:5" s="1" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="2:5" s="1" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B9" s="12">
         <v>1</v>
       </c>
@@ -1242,7 +1242,7 @@
       <c r="D9" s="16"/>
       <c r="E9" s="10"/>
     </row>
-    <row r="10" spans="2:5" s="1" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="2:5" s="1" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B10" s="12">
         <v>0</v>
       </c>
@@ -1252,7 +1252,7 @@
       <c r="D10" s="16"/>
       <c r="E10" s="10"/>
     </row>
-    <row r="11" spans="2:5" s="1" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="2:5" s="1" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B11" s="12">
         <f>AVERAGE(B12:B12)</f>
         <v>1</v>
@@ -1263,7 +1263,7 @@
       <c r="D11" s="16"/>
       <c r="E11" s="10"/>
     </row>
-    <row r="12" spans="2:5" s="1" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="2:5" s="1" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B12" s="12">
         <v>1</v>
       </c>
@@ -1273,7 +1273,7 @@
       <c r="D12" s="16"/>
       <c r="E12" s="10"/>
     </row>
-    <row r="13" spans="2:5" s="1" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="2:5" s="1" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B13" s="12">
         <f>AVERAGE(B14:B16)</f>
         <v>1</v>
@@ -1284,7 +1284,7 @@
       <c r="D13" s="16"/>
       <c r="E13" s="10"/>
     </row>
-    <row r="14" spans="2:5" s="1" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="2:5" s="1" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B14" s="12">
         <v>1</v>
       </c>
@@ -1294,7 +1294,7 @@
       <c r="D14" s="16"/>
       <c r="E14" s="10"/>
     </row>
-    <row r="15" spans="2:5" s="1" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="2:5" s="1" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B15" s="12">
         <v>1</v>
       </c>
@@ -1304,7 +1304,7 @@
       <c r="D15" s="16"/>
       <c r="E15" s="10"/>
     </row>
-    <row r="16" spans="2:5" s="1" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="2:5" s="1" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B16" s="23">
         <v>1</v>
       </c>
@@ -1314,7 +1314,7 @@
       <c r="D16" s="16"/>
       <c r="E16" s="10"/>
     </row>
-    <row r="17" spans="2:5" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="2:5" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B17" s="12">
         <f>AVERAGE(B18:B22)</f>
         <v>1</v>
@@ -1325,7 +1325,7 @@
       <c r="D17" s="16"/>
       <c r="E17" s="10"/>
     </row>
-    <row r="18" spans="2:5" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="2:5" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B18" s="12">
         <v>1</v>
       </c>
@@ -1335,7 +1335,7 @@
       <c r="D18" s="16"/>
       <c r="E18" s="10"/>
     </row>
-    <row r="19" spans="2:5" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="2:5" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B19" s="12">
         <v>1</v>
       </c>
@@ -1345,7 +1345,7 @@
       <c r="D19" s="16"/>
       <c r="E19" s="10"/>
     </row>
-    <row r="20" spans="2:5" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="2:5" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B20" s="12">
         <v>1</v>
       </c>
@@ -1355,7 +1355,7 @@
       <c r="D20" s="16"/>
       <c r="E20" s="10"/>
     </row>
-    <row r="21" spans="2:5" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="2:5" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B21" s="23">
         <v>1</v>
       </c>
@@ -1365,7 +1365,7 @@
       <c r="D21" s="16"/>
       <c r="E21" s="10"/>
     </row>
-    <row r="22" spans="2:5" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="2:5" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B22" s="23">
         <v>1</v>
       </c>
@@ -1375,7 +1375,7 @@
       <c r="D22" s="16"/>
       <c r="E22" s="10"/>
     </row>
-    <row r="23" spans="2:5" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="2:5" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B23" s="23">
         <f>AVERAGE(B24:B25)</f>
         <v>1</v>
@@ -1386,7 +1386,7 @@
       <c r="D23" s="16"/>
       <c r="E23" s="10"/>
     </row>
-    <row r="24" spans="2:5" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="2:5" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B24" s="23">
         <v>1</v>
       </c>
@@ -1396,7 +1396,7 @@
       <c r="D24" s="16"/>
       <c r="E24" s="10"/>
     </row>
-    <row r="25" spans="2:5" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="2:5" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B25" s="23">
         <v>1</v>
       </c>
@@ -1456,22 +1456,22 @@
   </sheetPr>
   <dimension ref="B1:E17"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="B8" workbookViewId="0">
-      <selection activeCell="E15" sqref="E15"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="B15" workbookViewId="0">
+      <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="9.125" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="2.7109375" customWidth="1"/>
-    <col min="2" max="2" width="15.7109375" customWidth="1"/>
-    <col min="3" max="3" width="30.7109375" customWidth="1"/>
-    <col min="4" max="4" width="15.7109375" customWidth="1"/>
-    <col min="5" max="5" width="53.5703125" customWidth="1"/>
-    <col min="6" max="6" width="2.7109375" customWidth="1"/>
-    <col min="8" max="8" width="9.140625" customWidth="1"/>
+    <col min="1" max="1" width="2.75" customWidth="1"/>
+    <col min="2" max="2" width="15.75" customWidth="1"/>
+    <col min="3" max="3" width="30.75" customWidth="1"/>
+    <col min="4" max="4" width="15.75" customWidth="1"/>
+    <col min="5" max="5" width="53.625" customWidth="1"/>
+    <col min="6" max="6" width="2.75" customWidth="1"/>
+    <col min="8" max="8" width="9.125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:5" s="1" customFormat="1" ht="42.75" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="2:5" s="1" customFormat="1" ht="42.75" customHeight="1" x14ac:dyDescent="0.5">
       <c r="B1" s="9" t="str">
         <f>Title</f>
         <v>STAR TREK ADVENTURES RULESET</v>
@@ -1480,8 +1480,8 @@
       <c r="D1" s="9"/>
       <c r="E1" s="9"/>
     </row>
-    <row r="2" spans="2:5" ht="15" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="3" spans="2:5" s="1" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="2:5" ht="15" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="3" spans="2:5" s="1" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B3" s="29" t="s">
         <v>0</v>
       </c>
@@ -1491,7 +1491,7 @@
       </c>
       <c r="E3" s="27"/>
     </row>
-    <row r="4" spans="2:5" s="1" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:5" s="1" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B4" s="29" t="s">
         <v>1</v>
       </c>
@@ -1499,8 +1499,8 @@
       <c r="D4" s="28"/>
       <c r="E4" s="28"/>
     </row>
-    <row r="5" spans="2:5" ht="15" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="6" spans="2:5" s="1" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:5" ht="15" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="6" spans="2:5" s="1" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B6" s="30" t="s">
         <v>25</v>
       </c>
@@ -1508,7 +1508,7 @@
       <c r="D6" s="30"/>
       <c r="E6" s="30"/>
     </row>
-    <row r="7" spans="2:5" s="1" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="2:5" s="1" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B7" s="8" t="s">
         <v>4</v>
       </c>
@@ -1522,7 +1522,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="8" spans="2:5" s="1" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="2:5" s="1" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B8" s="13">
         <v>1</v>
       </c>
@@ -1534,7 +1534,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="9" spans="2:5" s="1" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="2:5" s="1" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B9" s="14">
         <v>1</v>
       </c>
@@ -1546,7 +1546,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="10" spans="2:5" s="1" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="2:5" s="1" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B10" s="14">
         <v>1</v>
       </c>
@@ -1558,7 +1558,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="11" spans="2:5" s="1" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="2:5" s="1" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B11" s="14">
         <v>1</v>
       </c>
@@ -1570,7 +1570,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="12" spans="2:5" s="1" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="2:5" s="1" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B12" s="14">
         <v>1</v>
       </c>
@@ -1582,7 +1582,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="13" spans="2:5" s="1" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="2:5" s="1" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B13" s="14">
         <v>1</v>
       </c>
@@ -1594,7 +1594,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="14" spans="2:5" s="1" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="2:5" s="1" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B14" s="14">
         <v>1</v>
       </c>
@@ -1606,9 +1606,9 @@
         <v>36</v>
       </c>
     </row>
-    <row r="15" spans="2:5" s="1" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="2:5" s="1" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B15" s="14">
-        <v>0.75</v>
+        <v>1</v>
       </c>
       <c r="C15" s="4" t="s">
         <v>37</v>
@@ -1618,9 +1618,9 @@
         <v>38</v>
       </c>
     </row>
-    <row r="16" spans="2:5" s="1" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="2:5" s="1" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B16" s="14">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C16" s="4" t="s">
         <v>37</v>
@@ -1630,9 +1630,9 @@
         <v>39</v>
       </c>
     </row>
-    <row r="17" spans="2:5" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="2:5" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B17" s="24">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C17" s="4" t="s">
         <v>37</v>
@@ -1696,18 +1696,18 @@
       <selection activeCell="A7" sqref="A7:XFD7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="9.125" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="2.7109375" customWidth="1"/>
-    <col min="2" max="2" width="15.7109375" customWidth="1"/>
-    <col min="3" max="3" width="30.7109375" customWidth="1"/>
-    <col min="4" max="4" width="15.7109375" customWidth="1"/>
-    <col min="5" max="5" width="53.5703125" customWidth="1"/>
-    <col min="6" max="6" width="2.7109375" customWidth="1"/>
-    <col min="8" max="8" width="9.140625" customWidth="1"/>
+    <col min="1" max="1" width="2.75" customWidth="1"/>
+    <col min="2" max="2" width="15.75" customWidth="1"/>
+    <col min="3" max="3" width="30.75" customWidth="1"/>
+    <col min="4" max="4" width="15.75" customWidth="1"/>
+    <col min="5" max="5" width="53.625" customWidth="1"/>
+    <col min="6" max="6" width="2.75" customWidth="1"/>
+    <col min="8" max="8" width="9.125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:5" s="1" customFormat="1" ht="42.75" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="2:5" s="1" customFormat="1" ht="42.75" customHeight="1" x14ac:dyDescent="0.5">
       <c r="B1" s="9" t="str">
         <f>Title</f>
         <v>STAR TREK ADVENTURES RULESET</v>
@@ -1716,8 +1716,8 @@
       <c r="D1" s="9"/>
       <c r="E1" s="9"/>
     </row>
-    <row r="2" spans="2:5" ht="15" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="3" spans="2:5" s="1" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="2:5" ht="15" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="3" spans="2:5" s="1" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B3" s="29" t="s">
         <v>0</v>
       </c>
@@ -1727,7 +1727,7 @@
       </c>
       <c r="E3" s="27"/>
     </row>
-    <row r="4" spans="2:5" s="1" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:5" s="1" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B4" s="29" t="s">
         <v>1</v>
       </c>
@@ -1735,8 +1735,8 @@
       <c r="D4" s="28"/>
       <c r="E4" s="28"/>
     </row>
-    <row r="5" spans="2:5" ht="15" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="6" spans="2:5" s="1" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:5" ht="15" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="6" spans="2:5" s="1" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B6" s="30" t="s">
         <v>26</v>
       </c>
@@ -1744,7 +1744,7 @@
       <c r="D6" s="30"/>
       <c r="E6" s="30"/>
     </row>
-    <row r="7" spans="2:5" s="1" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="2:5" s="1" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B7" s="8" t="s">
         <v>4</v>
       </c>
@@ -1758,55 +1758,55 @@
         <v>3</v>
       </c>
     </row>
-    <row r="8" spans="2:5" s="1" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="2:5" s="1" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B8" s="13"/>
       <c r="C8" s="2"/>
       <c r="D8" s="17"/>
       <c r="E8" s="3"/>
     </row>
-    <row r="9" spans="2:5" s="1" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="2:5" s="1" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B9" s="14"/>
       <c r="C9" s="4"/>
       <c r="D9" s="18"/>
       <c r="E9" s="5"/>
     </row>
-    <row r="10" spans="2:5" s="1" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="2:5" s="1" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B10" s="14"/>
       <c r="C10" s="4"/>
       <c r="D10" s="18"/>
       <c r="E10" s="5"/>
     </row>
-    <row r="11" spans="2:5" s="1" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="2:5" s="1" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B11" s="14"/>
       <c r="C11" s="4"/>
       <c r="D11" s="18"/>
       <c r="E11" s="5"/>
     </row>
-    <row r="12" spans="2:5" s="1" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="2:5" s="1" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B12" s="14"/>
       <c r="C12" s="4"/>
       <c r="D12" s="18"/>
       <c r="E12" s="5"/>
     </row>
-    <row r="13" spans="2:5" s="1" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="2:5" s="1" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B13" s="14"/>
       <c r="C13" s="4"/>
       <c r="D13" s="18"/>
       <c r="E13" s="5"/>
     </row>
-    <row r="14" spans="2:5" s="1" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="2:5" s="1" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B14" s="14"/>
       <c r="C14" s="4"/>
       <c r="D14" s="18"/>
       <c r="E14" s="5"/>
     </row>
-    <row r="15" spans="2:5" s="1" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="2:5" s="1" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B15" s="14"/>
       <c r="C15" s="4"/>
       <c r="D15" s="18"/>
       <c r="E15" s="5"/>
     </row>
-    <row r="16" spans="2:5" s="1" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="2:5" s="1" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B16" s="15"/>
       <c r="C16" s="6"/>
       <c r="D16" s="19"/>

</xml_diff>